<commit_message>
# Conclusions 42 - 4 layer - 'relu', 'relu' widths and batches around 200, 200 - relu relu with 200 200 is the best option - test accuracy 0.9840 (rest are a bit less) ### Conclusions going forward: - So far for 4 layers relu relu with 200 200 is the best option (accuracy .9840) - Wait for results of 4 layers with higher width than 300 - Wait for results of 5 layers with different parameters
</commit_message>
<xml_diff>
--- a/output/41_4_layers_different_widths_batches_funcs/best.xlsx
+++ b/output/41_4_layers_different_widths_batches_funcs/best.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rkrichev\Documents\Yoni\DataScience\data-science-ml-dl-mnist\output\41_4_layers_different_widths_batches_funcs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -100,8 +105,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,10 +158,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -164,6 +175,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -210,7 +229,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -242,9 +261,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -276,6 +296,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -451,90 +472,96 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:23">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:23" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5.1068</v>
+        <v>5.1067999999999998</v>
       </c>
       <c r="C2">
-        <v>0.9847</v>
+        <v>0.98470000000000002</v>
       </c>
       <c r="D2">
         <v>200</v>
@@ -546,7 +573,7 @@
         <v>200</v>
       </c>
       <c r="G2">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="H2">
         <v>20.2578</v>
@@ -567,19 +594,19 @@
         <v>1</v>
       </c>
       <c r="N2">
-        <v>0.9847000241279602</v>
+        <v>0.98470002412796021</v>
       </c>
       <c r="O2">
-        <v>0.0844</v>
+        <v>8.4400000000000003E-2</v>
       </c>
       <c r="P2">
         <v>1</v>
       </c>
       <c r="Q2">
-        <v>0.0003</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="R2">
-        <v>240.021</v>
+        <v>240.02099999999999</v>
       </c>
       <c r="S2" t="s">
         <v>24</v>
@@ -591,21 +618,21 @@
         <v>0</v>
       </c>
       <c r="V2">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="W2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5.1902</v>
+        <v>5.1901999999999999</v>
       </c>
       <c r="C3">
-        <v>0.0708</v>
+        <v>7.0800000000000002E-2</v>
       </c>
       <c r="D3">
         <v>300</v>
@@ -617,10 +644,10 @@
         <v>300</v>
       </c>
       <c r="G3">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="H3">
-        <v>17.6383</v>
+        <v>17.638300000000001</v>
       </c>
       <c r="I3">
         <v>1000</v>
@@ -638,19 +665,19 @@
         <v>1</v>
       </c>
       <c r="N3">
-        <v>0.9830999970436096</v>
+        <v>0.98309999704360962</v>
       </c>
       <c r="O3">
-        <v>0.0708</v>
+        <v>7.0800000000000002E-2</v>
       </c>
       <c r="P3">
         <v>1</v>
       </c>
       <c r="Q3">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="R3">
-        <v>249.129</v>
+        <v>249.12899999999999</v>
       </c>
       <c r="S3" t="s">
         <v>25</v>
@@ -659,21 +686,21 @@
         <v>1</v>
       </c>
       <c r="U3">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="V3">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="W3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5.1248</v>
+        <v>5.1247999999999996</v>
       </c>
       <c r="C4">
         <v>11.83</v>
@@ -688,7 +715,7 @@
         <v>300</v>
       </c>
       <c r="G4">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="H4">
         <v>11.83</v>
@@ -712,28 +739,28 @@
         <v>0.982200026512146</v>
       </c>
       <c r="O4">
-        <v>0.0796</v>
+        <v>7.9600000000000004E-2</v>
       </c>
       <c r="P4">
-        <v>0.9980999827384949</v>
+        <v>0.99809998273849487</v>
       </c>
       <c r="Q4">
-        <v>0.0056</v>
+        <v>5.5999999999999999E-3</v>
       </c>
       <c r="R4">
-        <v>148.618</v>
+        <v>148.61799999999999</v>
       </c>
       <c r="S4" t="s">
         <v>26</v>
       </c>
       <c r="T4">
-        <v>0.9984999895095825</v>
+        <v>0.99849998950958252</v>
       </c>
       <c r="U4">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="V4">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="W4">
         <v>10</v>

</xml_diff>